<commit_message>
matching first and second code chunk
</commit_message>
<xml_diff>
--- a/Artists/ComeOnEileen.xlsx
+++ b/Artists/ComeOnEileen.xlsx
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Bridge 1</t>
+          <t>Pre-or-Post-Chorus 1</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Bridge 2</t>
+          <t>Pre-or-Post-Chorus 2</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Bridge 3</t>
+          <t>Pre-or-Post-Chorus 3</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -688,7 +688,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Bridge 4</t>
+          <t>Pre-or-Post-Chorus 4</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -700,7 +700,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Bridge 5</t>
+          <t>Pre-or-Post-Chorus 5</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -712,7 +712,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Bridge 6</t>
+          <t>Pre-or-Post-Chorus 6</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Bridge 7</t>
+          <t>Pre-or-Post-Chorus 7</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -736,7 +736,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Bridge 8</t>
+          <t>Pre-or-Post-Chorus 8</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -748,7 +748,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Bridge 9</t>
+          <t>Pre-or-Post-Chorus 9</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -760,7 +760,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Bridge 10</t>
+          <t>Pre-or-Post-Chorus 10</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -772,7 +772,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Bridge 11</t>
+          <t>Pre-or-Post-Chorus 11</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Bridge 12</t>
+          <t>Pre-or-Post-Chorus 12</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -796,7 +796,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Bridge 13</t>
+          <t>Pre-or-Post-Chorus 13</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Bridge 14</t>
+          <t>Pre-or-Post-Chorus 14</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -820,7 +820,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Bridge 15</t>
+          <t>Pre-or-Post-Chorus 15</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -832,7 +832,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Bridge 16</t>
+          <t>Pre-or-Post-Chorus 16</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -844,7 +844,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Bridge 17</t>
+          <t>Pre-or-Post-Chorus 17</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -856,7 +856,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Bridge 18</t>
+          <t>Pre-or-Post-Chorus 18</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -868,7 +868,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Bridge 19</t>
+          <t>Pre-or-Post-Chorus 19</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -880,7 +880,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Bridge 20</t>
+          <t>Pre-or-Post-Chorus 20</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -892,7 +892,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Bridge 21</t>
+          <t>Pre-or-Post-Chorus 21</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -904,7 +904,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Bridge 22</t>
+          <t>Pre-or-Post-Chorus 22</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -916,7 +916,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Bridge 23</t>
+          <t>Pre-or-Post-Chorus 23</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">

</xml_diff>